<commit_message>
* Added ability to double click on a record for jumping in the next stage (Aggregated level to Sample level and Sample level to Analytical Res. level), * Last modifications to table schema for Random genotyping records.
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.1.2.4.xlsx
+++ b/compat/tablesSchema.1.2.4.xlsx
@@ -24,8 +24,142 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SHAHAJ Alban</author>
+  </authors>
+  <commentList>
+    <comment ref="L8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+BSE (before)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Before:
+IF((%type.code==RGT),,AT06A)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Before:
+IF((%type.code==RGT),,AT06A)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+before:
+IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+before:
+IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,def</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="478">
   <si>
     <t>Type</t>
   </si>
@@ -1140,9 +1274,6 @@
     <t>IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
   </si>
   <si>
-    <t>IF((%type.code!=RGT),tseTargetGroup=%tseTargetGroup.code$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,)</t>
-  </si>
-  <si>
     <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),F02.A06AM,F02.A06AL)</t>
   </si>
   <si>
@@ -1338,24 +1469,15 @@
     <t>Sex of the animals</t>
   </si>
   <si>
-    <t>BSE</t>
-  </si>
-  <si>
     <t>%type.code|$%anMethType.code</t>
   </si>
   <si>
-    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)</t>
-  </si>
-  <si>
     <t>(%type.code==SCRAPIE)</t>
   </si>
   <si>
     <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
   </si>
   <si>
-    <t>IF((%type.code==RGT),,AT06A)</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -1459,6 +1581,15 @@
   </si>
   <si>
     <t>(%type.code==CWD)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),AT13A,AT06A)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)IF((%type.code==RGT),F089A,)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT),tseTargetGroup=%tseTargetGroup.code$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,totSamplesTested=%totSamplesTested.label)</t>
   </si>
   <si>
     <t>IF((%type.code!=RGT),SUM(%totSamplesPositive.label,%totSamplesNegative.label,%totSamplesInconclusive.label),)</t>
@@ -1468,7 +1599,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1501,6 +1632,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3819,10 +3963,10 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25:L42"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3939,16 +4083,16 @@
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
+        <v>429</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="27" t="s">
         <v>431</v>
       </c>
-      <c r="D3" s="27" t="s">
-        <v>432</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>12</v>
@@ -3966,16 +4110,16 @@
         <v>9</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>9</v>
@@ -4467,7 +4611,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="8" t="s">
@@ -4698,7 +4842,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="18"/>
       <c r="E8" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>174</v>
@@ -4729,13 +4873,13 @@
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>174</v>
@@ -4766,13 +4910,13 @@
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
       <c r="E10" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>174</v>
@@ -4810,10 +4954,10 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
@@ -4853,10 +4997,10 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>174</v>
@@ -4889,15 +5033,15 @@
     </row>
     <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>376</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>377</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>174</v>
@@ -4936,14 +5080,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomRight" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5100,13 +5244,13 @@
         <v>108</v>
       </c>
       <c r="L3" s="33" t="s">
+        <v>467</v>
+      </c>
+      <c r="M3" s="33" t="s">
         <v>471</v>
       </c>
-      <c r="M3" s="33" t="s">
-        <v>475</v>
-      </c>
       <c r="N3" s="33" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -5126,7 +5270,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>69</v>
@@ -5141,7 +5285,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>3</v>
@@ -5255,40 +5399,40 @@
     </row>
     <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>435</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>436</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="33" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L7" s="34" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="6" t="s">
@@ -5312,10 +5456,10 @@
         <v>89</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>12</v>
@@ -5335,14 +5479,14 @@
       <c r="K8" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>442</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>442</v>
+      <c r="L8" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="M8" s="33" t="s">
+        <v>474</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>474</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>9</v>
@@ -5365,10 +5509,10 @@
         <v>92</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>12</v>
@@ -5389,13 +5533,13 @@
         <v>112</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>438</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>439</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>439</v>
+        <v>436</v>
+      </c>
+      <c r="M9" s="33" t="s">
+        <v>475</v>
+      </c>
+      <c r="N9" s="33" t="s">
+        <v>475</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>9</v>
@@ -5415,7 +5559,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>36</v>
@@ -5427,10 +5571,10 @@
         <v>37</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>3</v>
@@ -5442,13 +5586,13 @@
         <v>312</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>5</v>
@@ -5462,23 +5606,23 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>202</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="33" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>3</v>
@@ -5530,9 +5674,7 @@
       <c r="R12" s="6">
         <v>11</v>
       </c>
-      <c r="S12" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="S12" s="33"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -5630,19 +5772,19 @@
         <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="P15" s="33" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -5700,7 +5842,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>174</v>
@@ -5718,7 +5860,7 @@
         <v>3</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>9</v>
@@ -5745,10 +5887,10 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>3</v>
@@ -5757,7 +5899,7 @@
         <v>319</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>5</v>
@@ -5787,10 +5929,10 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>3</v>
@@ -5799,7 +5941,7 @@
         <v>319</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>5</v>
@@ -5927,13 +6069,13 @@
         <v>4</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -6019,8 +6161,8 @@
       <c r="J26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P26" s="6" t="s">
-        <v>371</v>
+      <c r="P26" s="33" t="s">
+        <v>476</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>9</v>
@@ -6049,7 +6191,7 @@
         <v>4</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>3</v>
@@ -6171,7 +6313,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -6203,7 +6345,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>9</v>
@@ -6267,7 +6409,7 @@
         <v>4</v>
       </c>
       <c r="P34" s="6" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>9</v>
@@ -6299,7 +6441,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -6307,13 +6449,13 @@
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>417</v>
-      </c>
       <c r="C36" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>174</v>
@@ -6328,7 +6470,7 @@
         <v>4</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>9</v>
@@ -6395,7 +6537,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -6456,7 +6598,7 @@
         <v>4</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>9</v>
@@ -6520,8 +6662,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6621,13 +6764,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B2" t="s">
         <v>191</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>211</v>
@@ -6730,10 +6873,10 @@
         <v>303</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>372</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>373</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>5</v>
@@ -6747,40 +6890,40 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="J5" s="33" t="s">
         <v>3</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>397</v>
-      </c>
       <c r="M5" s="33" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -6809,19 +6952,19 @@
         <v>74</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>111</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>5</v>
@@ -6850,7 +6993,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>3</v>
@@ -6888,7 +7031,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>3</v>
@@ -7032,7 +7175,7 @@
         <v>217</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>3</v>
@@ -7073,10 +7216,10 @@
         <v>197</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>369</v>
@@ -7088,7 +7231,7 @@
         <v>303</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="N13" s="22"/>
       <c r="Q13" s="6" t="s">
@@ -7118,7 +7261,7 @@
         <v>42</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>3</v>
@@ -7158,7 +7301,7 @@
         <v>282</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>3</v>
@@ -7167,7 +7310,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -7194,7 +7337,7 @@
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>3</v>
@@ -7241,10 +7384,10 @@
         <v>3</v>
       </c>
       <c r="K17" s="20" t="s">
+        <v>432</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>433</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>434</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7403,10 +7546,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E24" activeCellId="1" sqref="E13:E14 E24"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7503,19 +7646,19 @@
         <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>319</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>5</v>
@@ -7541,19 +7684,19 @@
         <v>12</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>319</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -7594,7 +7737,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>294</v>
@@ -7629,7 +7772,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -7763,19 +7906,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>424</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>425</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>174</v>
@@ -7842,7 +7985,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>9</v>
@@ -7850,10 +7993,10 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>174</v>
@@ -7868,7 +8011,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -7926,7 +8069,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -7993,7 +8136,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>9</v>
@@ -8001,7 +8144,7 @@
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>174</v>
@@ -8019,7 +8162,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -8068,10 +8211,10 @@
         <v>11</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>174</v>
@@ -8089,7 +8232,7 @@
         <v>4</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>9</v>
@@ -8190,7 +8333,7 @@
         <v>95</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>256</v>
@@ -8246,7 +8389,7 @@
         <v>4</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>9</v>
@@ -8464,7 +8607,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -8510,13 +8653,13 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>417</v>
-      </c>
       <c r="C33" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>174</v>
@@ -8531,7 +8674,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -8595,7 +8738,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -8691,7 +8834,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -8699,13 +8842,13 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>420</v>
-      </c>
       <c r="C39" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>174</v>
@@ -8720,7 +8863,7 @@
         <v>4</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>9</v>
@@ -8763,7 +8906,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>57</v>
@@ -8781,7 +8924,7 @@
         <v>4</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>5</v>
@@ -9031,7 +9174,7 @@
         <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9039,7 +9182,7 @@
         <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9063,7 +9206,7 @@
         <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -9071,7 +9214,7 @@
         <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -9438,7 +9581,7 @@
         <v>361</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
@@ -9494,7 +9637,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>344</v>

</xml_diff>

<commit_message>
* solved other bugs related with status Valid with Warning
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.1.2.4.xlsx
+++ b/compat/tablesSchema.1.2.4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20070" windowHeight="3840" tabRatio="690" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="20070" windowHeight="3780" tabRatio="690" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -154,12 +154,288 @@
         </r>
       </text>
     </comment>
+    <comment ref="M10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+empty</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),Not infected,)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SHAHAJ Alban</author>
+  </authors>
+  <commentList>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+(RELATION{SummarizedInformation,type.code}!=RGT)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+(RELATION{SummarizedInformation,type.code}==RGT)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+(RELATION{SummarizedInformation,type.code}!=RGT)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+AND((RELATION{SummarizedInformation,type.code}!=BSE),(%sampEventAsses.code!=J051A))</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+(RELATION{SummarizedInformation,type.code}!=RGT)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+IF(AND((RELATION{SummarizedInformation,type.code}==BSE),(%sampEventAsses.code!=J051A)),Y,)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+IF(AND((RELATION{SummarizedInformation,type.code}==BSE),(%sampEventAsses.code!=J051A)),Y,)
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="476">
   <si>
     <t>Type</t>
   </si>
@@ -1520,9 +1796,6 @@
     <t>%progId.label</t>
   </si>
   <si>
-    <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),Not infected,)</t>
-  </si>
-  <si>
     <t>NEXT(,)</t>
   </si>
   <si>
@@ -1556,12 +1829,6 @@
     <t>IF((%type.code==RGT),0,)</t>
   </si>
   <si>
-    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=BSE))</t>
-  </si>
-  <si>
-    <t>IF(AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}==BSE)),Y,)</t>
-  </si>
-  <si>
     <t>%type.code|IF((%type.code==CWD),$RELATION{Preferences,cwdExtCont.label},)</t>
   </si>
   <si>
@@ -1593,6 +1860,9 @@
   </si>
   <si>
     <t>IF((%type.code!=RGT),SUM(%totSamplesPositive.label,%totSamplesNegative.label,%totSamplesInconclusive.label),)</t>
+  </si>
+  <si>
+    <t>IF(AND((RELATION{SummarizedInformation,type.code}==BSE),(%sampEventAsses.code!=J051A)),Y,)</t>
   </si>
 </sst>
 </file>
@@ -1662,13 +1932,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1776,9 +2046,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1786,9 +2054,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3746,7 +4018,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4082,37 +4354,37 @@
       </c>
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="24" t="s">
         <v>429</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>431</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="27" t="s">
+      <c r="J3" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="25" t="s">
         <v>432</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="26" t="s">
         <v>440</v>
       </c>
       <c r="M3" s="17" t="s">
@@ -4373,25 +4645,25 @@
       <c r="E10" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="27" t="s">
         <v>93</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="29" t="s">
+      <c r="I10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="L10" s="28" t="s">
         <v>355</v>
       </c>
       <c r="R10" s="2">
@@ -4412,25 +4684,25 @@
       <c r="E11" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="27" t="s">
         <v>93</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11" s="29" t="s">
+      <c r="I11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="28" t="s">
         <v>356</v>
       </c>
       <c r="R11" s="2">
@@ -4451,25 +4723,25 @@
       <c r="E12" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="29" t="s">
         <v>93</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="31" t="s">
+      <c r="I12" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="28" t="s">
         <v>357</v>
       </c>
       <c r="M12" s="10"/>
@@ -4954,7 +5226,7 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>402</v>
@@ -4997,7 +5269,7 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>402</v>
@@ -5083,33 +5355,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S12" sqref="S12"/>
+      <selection pane="bottomRight" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="6"/>
+    <col min="2" max="2" width="7.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="6" customWidth="1"/>
     <col min="5" max="5" width="40" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="39" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="68.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.5703125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="74.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.85546875" style="6" customWidth="1"/>
     <col min="14" max="14" width="50.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" style="6" customWidth="1"/>
     <col min="16" max="16" width="52.5703125" style="6" customWidth="1"/>
     <col min="17" max="17" width="9.85546875" style="6" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="6"/>
+    <col min="18" max="18" width="9.140625" style="6"/>
+    <col min="19" max="19" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -5243,14 +5516,14 @@
       <c r="K3" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="33" t="s">
-        <v>467</v>
-      </c>
-      <c r="M3" s="33" t="s">
-        <v>471</v>
-      </c>
-      <c r="N3" s="33" t="s">
-        <v>471</v>
+      <c r="L3" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="N3" s="30" t="s">
+        <v>468</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -5397,7 +5670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>390</v>
       </c>
@@ -5419,8 +5692,8 @@
       <c r="H7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="33" t="s">
-        <v>473</v>
+      <c r="I7" s="30" t="s">
+        <v>470</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>3</v>
@@ -5428,11 +5701,11 @@
       <c r="K7" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="L7" s="34" t="s">
-        <v>467</v>
+      <c r="L7" s="31" t="s">
+        <v>464</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="6" t="s">
@@ -5479,14 +5752,14 @@
       <c r="K8" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="30" t="s">
         <v>312</v>
       </c>
-      <c r="M8" s="33" t="s">
-        <v>474</v>
-      </c>
-      <c r="N8" s="33" t="s">
-        <v>474</v>
+      <c r="M8" s="30" t="s">
+        <v>471</v>
+      </c>
+      <c r="N8" s="30" t="s">
+        <v>471</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>9</v>
@@ -5535,11 +5808,11 @@
       <c r="L9" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="M9" s="33" t="s">
-        <v>475</v>
-      </c>
-      <c r="N9" s="33" t="s">
-        <v>475</v>
+      <c r="M9" s="30" t="s">
+        <v>472</v>
+      </c>
+      <c r="N9" s="30" t="s">
+        <v>472</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>9</v>
@@ -5585,15 +5858,12 @@
       <c r="L10" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="32"/>
+      <c r="N10" s="32" t="s">
         <v>450</v>
       </c>
-      <c r="O10" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>453</v>
-      </c>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
       <c r="Q10" s="6" t="s">
         <v>5</v>
       </c>
@@ -5605,7 +5875,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>408</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -5618,11 +5888,11 @@
         <v>174</v>
       </c>
       <c r="G11" s="17"/>
-      <c r="H11" s="33" t="s">
-        <v>472</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>472</v>
+      <c r="H11" s="30" t="s">
+        <v>469</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>469</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>3</v>
@@ -5674,7 +5944,6 @@
       <c r="R12" s="6">
         <v>11</v>
       </c>
-      <c r="S12" s="33"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -5772,19 +6041,19 @@
         <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>464</v>
-      </c>
-      <c r="P15" s="33" t="s">
-        <v>477</v>
+        <v>463</v>
+      </c>
+      <c r="P15" s="30" t="s">
+        <v>474</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -5860,7 +6129,7 @@
         <v>3</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>9</v>
@@ -5887,10 +6156,10 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>3</v>
@@ -5899,7 +6168,7 @@
         <v>319</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>5</v>
@@ -5929,10 +6198,10 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>3</v>
@@ -5941,7 +6210,7 @@
         <v>319</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>5</v>
@@ -6069,13 +6338,13 @@
         <v>4</v>
       </c>
       <c r="M23" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="P23" s="6" t="s">
         <v>462</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>463</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -6161,8 +6430,8 @@
       <c r="J26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P26" s="33" t="s">
-        <v>476</v>
+      <c r="P26" s="30" t="s">
+        <v>473</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>9</v>
@@ -6470,7 +6739,7 @@
         <v>4</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>9</v>
@@ -6670,14 +6939,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6787,8 +7056,8 @@
       <c r="I2" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>369</v>
+      <c r="J2" s="32" t="s">
+        <v>3</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>212</v>
@@ -6910,10 +7179,10 @@
       <c r="H5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="32" t="s">
-        <v>469</v>
-      </c>
-      <c r="J5" s="33" t="s">
+      <c r="I5" s="33" t="s">
+        <v>466</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K5" s="6" t="s">
@@ -6922,8 +7191,8 @@
       <c r="L5" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="M5" s="33" t="s">
-        <v>470</v>
+      <c r="M5" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -6957,8 +7226,8 @@
       <c r="I6" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>397</v>
+      <c r="J6" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>111</v>
@@ -6998,8 +7267,8 @@
       <c r="I7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>369</v>
+      <c r="J7" s="32" t="s">
+        <v>3</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>5</v>
@@ -7196,7 +7465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>194</v>
       </c>
@@ -7215,14 +7484,14 @@
       <c r="G13" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>425</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>465</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>369</v>
+      <c r="H13" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="32" t="s">
+        <v>3</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>198</v>
@@ -7230,10 +7499,11 @@
       <c r="L13" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="M13" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="N13" s="22"/>
+      <c r="N13" s="34" t="s">
+        <v>475</v>
+      </c>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
       <c r="Q13" s="6" t="s">
         <v>5</v>
       </c>
@@ -7535,8 +7805,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7546,10 +7817,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8011,7 +8282,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -8674,7 +8945,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -9577,7 +9848,7 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="24" t="s">
+      <c r="P10" s="4" t="s">
         <v>361</v>
       </c>
       <c r="Q10" s="2" t="s">
@@ -9647,7 +9918,7 @@
       <c r="A13" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>315</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -9671,7 +9942,7 @@
       <c r="C14" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>315</v>
       </c>
       <c r="F14" s="2" t="s">

</xml_diff>